<commit_message>
Add control point study
</commit_message>
<xml_diff>
--- a/registration-params/process-results/results/registratrion-v4.xlsx
+++ b/registration-params/process-results/results/registratrion-v4.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Master thesis\master\registration-params\process-results\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4FB4B9-DCF5-4332-962B-8FE4AAA4CDE1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA774DD-AF68-4B26-BA0E-0B9EFEA5EBAC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{04B43123-9A0F-42C4-83EF-9ABEAD4EC2A2}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="5" xr2:uid="{04B43123-9A0F-42C4-83EF-9ABEAD4EC2A2}"/>
   </bookViews>
   <sheets>
     <sheet name="init" sheetId="9" r:id="rId1"/>
-    <sheet name="normal-linear-reg" sheetId="1" r:id="rId2"/>
-    <sheet name="sirt-linear-reg" sheetId="2" r:id="rId3"/>
-    <sheet name="sirt-deformable-reg" sheetId="8" r:id="rId4"/>
-    <sheet name="sirt-linear-deformable-reg" sheetId="10" r:id="rId5"/>
-    <sheet name="analysis-1" sheetId="5" r:id="rId6"/>
+    <sheet name="n-lin-reg" sheetId="1" r:id="rId2"/>
+    <sheet name="sirt-lin-reg" sheetId="2" r:id="rId3"/>
+    <sheet name="sirt-def-reg" sheetId="8" r:id="rId4"/>
+    <sheet name="sirt-lin-def-reg" sheetId="10" r:id="rId5"/>
+    <sheet name="sub-study" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="30">
   <si>
     <t>Rigid</t>
   </si>
@@ -108,6 +108,24 @@
   </si>
   <si>
     <t>Using liver segmentations</t>
+  </si>
+  <si>
+    <t>Point control study</t>
+  </si>
+  <si>
+    <t>Pat.</t>
+  </si>
+  <si>
+    <t>Deformation control points</t>
+  </si>
+  <si>
+    <t>Registration execution time</t>
+  </si>
+  <si>
+    <t>Average execution time</t>
+  </si>
+  <si>
+    <t>Average landmark distance error</t>
   </si>
 </sst>
 </file>
@@ -182,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -405,6 +423,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -414,7 +441,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -563,7 +590,6 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -651,6 +677,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1205,168 +1258,168 @@
   <dimension ref="B2:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M11"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="56"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1381,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5819BB-9216-4464-AEBA-067CE33D4444}">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:I13"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,38 +1455,38 @@
     <row r="2" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="21"/>
       <c r="C2" s="13"/>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="22"/>
       <c r="C3" s="14"/>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="64" t="s">
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="63"/>
-      <c r="I3" s="65"/>
-      <c r="N3" s="70" t="s">
+      <c r="H3" s="62"/>
+      <c r="I3" s="64"/>
+      <c r="N3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="71"/>
-      <c r="P3" s="72"/>
-      <c r="R3" s="66" t="s">
+      <c r="O3" s="70"/>
+      <c r="P3" s="71"/>
+      <c r="R3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
       <c r="U3" s="35">
         <v>20</v>
       </c>
@@ -1474,17 +1527,17 @@
       <c r="P4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="R4" s="66" t="s">
+      <c r="R4" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="66"/>
-      <c r="T4" s="66"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
       <c r="U4" s="35">
         <v>12.5</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="66" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="23">
@@ -1530,7 +1583,7 @@
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="14">
         <v>8</v>
       </c>
@@ -1574,7 +1627,7 @@
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="68"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14">
         <v>10</v>
       </c>
@@ -1618,7 +1671,7 @@
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="68"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="14">
         <v>11</v>
       </c>
@@ -1662,7 +1715,7 @@
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="68"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="14">
         <v>13</v>
       </c>
@@ -1706,7 +1759,7 @@
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="68"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="14">
         <v>20</v>
       </c>
@@ -1750,7 +1803,7 @@
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="68"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="14">
         <v>21</v>
       </c>
@@ -1794,7 +1847,7 @@
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="68"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="14">
         <v>22</v>
       </c>
@@ -1838,7 +1891,7 @@
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="68"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="14">
         <v>23</v>
       </c>
@@ -1882,7 +1935,7 @@
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="68"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="14">
         <v>25</v>
       </c>
@@ -1926,7 +1979,7 @@
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="68"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="14">
         <v>26</v>
       </c>
@@ -1970,7 +2023,7 @@
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="68"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="14">
         <v>28</v>
       </c>
@@ -2014,7 +2067,7 @@
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="68"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="14">
         <v>30</v>
       </c>
@@ -2058,7 +2111,7 @@
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="68"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="14">
         <v>34</v>
       </c>
@@ -2101,7 +2154,7 @@
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="68"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="14">
         <v>36</v>
       </c>
@@ -2145,7 +2198,7 @@
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="68"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="14">
         <v>37</v>
       </c>
@@ -2189,7 +2242,7 @@
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="68"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="14">
         <v>40</v>
       </c>
@@ -2233,7 +2286,7 @@
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="68"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="14">
         <v>41</v>
       </c>
@@ -2277,7 +2330,7 @@
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="68"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="14">
         <v>46</v>
       </c>
@@ -2321,7 +2374,7 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="68"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="14">
         <v>49</v>
       </c>
@@ -2365,7 +2418,7 @@
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="68"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="14">
         <v>50</v>
       </c>
@@ -2408,7 +2461,7 @@
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="68"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="14">
         <v>55</v>
       </c>
@@ -2451,7 +2504,7 @@
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="68"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="14">
         <v>56</v>
       </c>
@@ -2495,7 +2548,7 @@
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="68"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="14">
         <v>62</v>
       </c>
@@ -2539,7 +2592,7 @@
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="68"/>
+      <c r="B29" s="67"/>
       <c r="C29" s="14">
         <v>66</v>
       </c>
@@ -2583,7 +2636,7 @@
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="68"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="14">
         <v>67</v>
       </c>
@@ -2627,7 +2680,7 @@
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="68"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="14">
         <v>69</v>
       </c>
@@ -2671,7 +2724,7 @@
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="68"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="14">
         <v>70</v>
       </c>
@@ -2715,7 +2768,7 @@
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="68"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="14">
         <v>71</v>
       </c>
@@ -2759,7 +2812,7 @@
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="14">
         <v>74</v>
       </c>
@@ -2803,7 +2856,7 @@
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="68"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="14">
         <v>75</v>
       </c>
@@ -2846,7 +2899,7 @@
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="68"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="14">
         <v>78</v>
       </c>
@@ -2890,7 +2943,7 @@
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="68"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="14">
         <v>79</v>
       </c>
@@ -2934,7 +2987,7 @@
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="68"/>
+      <c r="B38" s="67"/>
       <c r="C38" s="14">
         <v>80</v>
       </c>
@@ -2978,7 +3031,7 @@
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="68"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="14">
         <v>81</v>
       </c>
@@ -3022,7 +3075,7 @@
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="68"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="14">
         <v>82</v>
       </c>
@@ -3066,7 +3119,7 @@
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="68"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="14">
         <v>83</v>
       </c>
@@ -3110,7 +3163,7 @@
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="68"/>
+      <c r="B42" s="67"/>
       <c r="C42" s="14">
         <v>86</v>
       </c>
@@ -3154,7 +3207,7 @@
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="68"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="14">
         <v>88</v>
       </c>
@@ -3198,7 +3251,7 @@
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="68"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="14">
         <v>90</v>
       </c>
@@ -3242,7 +3295,7 @@
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="68"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="14">
         <v>91</v>
       </c>
@@ -3285,7 +3338,7 @@
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="68"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="14">
         <v>92</v>
       </c>
@@ -3329,7 +3382,7 @@
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="68"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="14">
         <v>93</v>
       </c>
@@ -3373,7 +3426,7 @@
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="68"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="14">
         <v>94</v>
       </c>
@@ -3417,7 +3470,7 @@
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B49" s="68"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="14">
         <v>95</v>
       </c>
@@ -3461,7 +3514,7 @@
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B50" s="68"/>
+      <c r="B50" s="67"/>
       <c r="C50" s="14">
         <v>96</v>
       </c>
@@ -3505,7 +3558,7 @@
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B51" s="68"/>
+      <c r="B51" s="67"/>
       <c r="C51" s="14">
         <v>97</v>
       </c>
@@ -3549,7 +3602,7 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B52" s="68"/>
+      <c r="B52" s="67"/>
       <c r="C52" s="14">
         <v>98</v>
       </c>
@@ -3593,7 +3646,7 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="68"/>
+      <c r="B53" s="67"/>
       <c r="C53" s="14">
         <v>99</v>
       </c>
@@ -3637,7 +3690,7 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="68"/>
+      <c r="B54" s="67"/>
       <c r="C54" s="14">
         <v>100</v>
       </c>
@@ -3681,7 +3734,7 @@
       </c>
     </row>
     <row r="55" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="69"/>
+      <c r="B55" s="68"/>
       <c r="C55" s="15">
         <v>103</v>
       </c>
@@ -3738,10 +3791,10 @@
     </row>
     <row r="57" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="36"/>
-      <c r="B57" s="58" t="s">
+      <c r="B57" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="58"/>
+      <c r="C57" s="57"/>
       <c r="D57" s="51">
         <f>+AVERAGEIF(D5:D55, "&lt;"&amp;$U$3)</f>
         <v>14.27243181818182</v>
@@ -3766,10 +3819,10 @@
         <v>20</v>
       </c>
       <c r="J57" s="36"/>
-      <c r="K57" s="58" t="s">
+      <c r="K57" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="L57" s="58"/>
+      <c r="L57" s="57"/>
       <c r="N57" s="9"/>
       <c r="O57" s="28" t="s">
         <v>0</v>
@@ -3780,10 +3833,10 @@
     </row>
     <row r="58" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="36"/>
-      <c r="B58" s="58" t="s">
+      <c r="B58" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="58"/>
+      <c r="C58" s="57"/>
       <c r="D58" s="51">
         <f t="array" ref="D58">_xlfn.STDEV.P(IF(D5:D55&lt;50,D5:D55))</f>
         <v>9.9427579475592918</v>
@@ -3809,11 +3862,11 @@
         <v>5.4527209990609693</v>
       </c>
       <c r="J58" s="36"/>
-      <c r="K58" s="58" t="str">
+      <c r="K58" s="57" t="str">
         <f>+_xlfn.CONCAT(COUNTIF(K5:K55, "&lt;"&amp;$U$4), "/", COUNT(K5:K55))</f>
         <v>7/31</v>
       </c>
-      <c r="L58" s="58"/>
+      <c r="L58" s="57"/>
       <c r="N58" s="33" t="s">
         <v>2</v>
       </c>
@@ -3828,10 +3881,10 @@
     </row>
     <row r="59" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="36"/>
-      <c r="B59" s="58" t="s">
+      <c r="B59" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="58"/>
+      <c r="C59" s="57"/>
       <c r="D59" s="47" t="str">
         <f t="shared" ref="D59:I59" si="9">+_xlfn.CONCAT(COUNTIF(D5:D55, "&gt;"&amp;$U$3), "/", COUNT(D5:D55))</f>
         <v>40/51</v>
@@ -3947,8 +4000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACC9F12-62F0-45B6-A857-447593DB2FC2}">
   <dimension ref="B1:U61"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:F6"/>
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3975,40 +4028,40 @@
     <row r="2" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11"/>
       <c r="C2" s="13"/>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
       <c r="C3" s="14"/>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="64" t="s">
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="63"/>
-      <c r="I3" s="65"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="64"/>
       <c r="K3"/>
       <c r="L3"/>
-      <c r="N3" s="70" t="s">
+      <c r="N3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="71"/>
-      <c r="P3" s="72"/>
-      <c r="R3" s="66" t="s">
+      <c r="O3" s="70"/>
+      <c r="P3" s="71"/>
+      <c r="R3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
       <c r="U3" s="35">
         <v>20</v>
       </c>
@@ -4049,17 +4102,17 @@
       <c r="P4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="R4" s="66" t="s">
+      <c r="R4" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="66"/>
-      <c r="T4" s="66"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
       <c r="U4" s="35">
         <v>12.5</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="67" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="14">
@@ -4105,7 +4158,7 @@
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="14">
         <v>8</v>
       </c>
@@ -4149,7 +4202,7 @@
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="68"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14">
         <v>10</v>
       </c>
@@ -4193,7 +4246,7 @@
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="68"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="14">
         <v>11</v>
       </c>
@@ -4237,7 +4290,7 @@
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="68"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="14">
         <v>13</v>
       </c>
@@ -4281,7 +4334,7 @@
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="68"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="14">
         <v>20</v>
       </c>
@@ -4325,7 +4378,7 @@
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="68"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="14">
         <v>21</v>
       </c>
@@ -4369,7 +4422,7 @@
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="68"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="14">
         <v>22</v>
       </c>
@@ -4413,7 +4466,7 @@
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="68"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="14">
         <v>23</v>
       </c>
@@ -4457,7 +4510,7 @@
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="68"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="14">
         <v>25</v>
       </c>
@@ -4501,7 +4554,7 @@
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="68"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="14">
         <v>26</v>
       </c>
@@ -4545,7 +4598,7 @@
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="68"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="14">
         <v>28</v>
       </c>
@@ -4589,7 +4642,7 @@
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="68"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="14">
         <v>30</v>
       </c>
@@ -4633,7 +4686,7 @@
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="68"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="14">
         <v>34</v>
       </c>
@@ -4677,7 +4730,7 @@
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="68"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="14">
         <v>36</v>
       </c>
@@ -4721,7 +4774,7 @@
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="68"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="14">
         <v>37</v>
       </c>
@@ -4765,7 +4818,7 @@
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="68"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="14">
         <v>40</v>
       </c>
@@ -4809,7 +4862,7 @@
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="68"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="14">
         <v>41</v>
       </c>
@@ -4853,7 +4906,7 @@
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="68"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="14">
         <v>46</v>
       </c>
@@ -4897,7 +4950,7 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="68"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="14">
         <v>49</v>
       </c>
@@ -4941,7 +4994,7 @@
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="68"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="14">
         <v>50</v>
       </c>
@@ -4985,7 +5038,7 @@
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="68"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="14">
         <v>55</v>
       </c>
@@ -5029,7 +5082,7 @@
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="68"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="14">
         <v>56</v>
       </c>
@@ -5073,7 +5126,7 @@
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="68"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="14">
         <v>62</v>
       </c>
@@ -5117,7 +5170,7 @@
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="68"/>
+      <c r="B29" s="67"/>
       <c r="C29" s="14">
         <v>66</v>
       </c>
@@ -5161,7 +5214,7 @@
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="68"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="14">
         <v>67</v>
       </c>
@@ -5205,7 +5258,7 @@
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="68"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="14">
         <v>69</v>
       </c>
@@ -5249,7 +5302,7 @@
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="68"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="14">
         <v>70</v>
       </c>
@@ -5293,7 +5346,7 @@
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="68"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="14">
         <v>71</v>
       </c>
@@ -5337,7 +5390,7 @@
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="14">
         <v>74</v>
       </c>
@@ -5381,7 +5434,7 @@
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="68"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="14">
         <v>75</v>
       </c>
@@ -5425,7 +5478,7 @@
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="68"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="14">
         <v>78</v>
       </c>
@@ -5469,7 +5522,7 @@
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="68"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="14">
         <v>79</v>
       </c>
@@ -5513,7 +5566,7 @@
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="68"/>
+      <c r="B38" s="67"/>
       <c r="C38" s="14">
         <v>80</v>
       </c>
@@ -5557,7 +5610,7 @@
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="68"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="14">
         <v>81</v>
       </c>
@@ -5601,7 +5654,7 @@
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="68"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="14">
         <v>82</v>
       </c>
@@ -5645,7 +5698,7 @@
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="68"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="14">
         <v>83</v>
       </c>
@@ -5689,7 +5742,7 @@
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="68"/>
+      <c r="B42" s="67"/>
       <c r="C42" s="14">
         <v>86</v>
       </c>
@@ -5733,7 +5786,7 @@
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="68"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="14">
         <v>88</v>
       </c>
@@ -5777,7 +5830,7 @@
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="68"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="14">
         <v>90</v>
       </c>
@@ -5821,7 +5874,7 @@
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="68"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="14">
         <v>91</v>
       </c>
@@ -5865,7 +5918,7 @@
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="68"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="14">
         <v>92</v>
       </c>
@@ -5909,7 +5962,7 @@
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="68"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="14">
         <v>93</v>
       </c>
@@ -5953,7 +6006,7 @@
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="68"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="14">
         <v>94</v>
       </c>
@@ -5997,7 +6050,7 @@
       </c>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B49" s="68"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="14">
         <v>95</v>
       </c>
@@ -6041,7 +6094,7 @@
       </c>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B50" s="68"/>
+      <c r="B50" s="67"/>
       <c r="C50" s="14">
         <v>96</v>
       </c>
@@ -6085,7 +6138,7 @@
       </c>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B51" s="68"/>
+      <c r="B51" s="67"/>
       <c r="C51" s="14">
         <v>97</v>
       </c>
@@ -6130,7 +6183,7 @@
       <c r="S51" s="9"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B52" s="68"/>
+      <c r="B52" s="67"/>
       <c r="C52" s="14">
         <v>98</v>
       </c>
@@ -6175,7 +6228,7 @@
       <c r="S52" s="9"/>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B53" s="68"/>
+      <c r="B53" s="67"/>
       <c r="C53" s="14">
         <v>99</v>
       </c>
@@ -6220,7 +6273,7 @@
       <c r="S53" s="9"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B54" s="68"/>
+      <c r="B54" s="67"/>
       <c r="C54" s="14">
         <v>100</v>
       </c>
@@ -6265,7 +6318,7 @@
       <c r="S54" s="9"/>
     </row>
     <row r="55" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="69"/>
+      <c r="B55" s="68"/>
       <c r="C55" s="15">
         <v>103</v>
       </c>
@@ -6321,10 +6374,10 @@
       <c r="L56" s="20"/>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B57" s="58" t="s">
+      <c r="B57" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="58"/>
+      <c r="C57" s="57"/>
       <c r="D57" s="51">
         <f t="shared" ref="D57:I57" si="10">+AVERAGEIF(D5:D55, "&lt;"&amp;$U$3)</f>
         <v>13.519419166666665</v>
@@ -6349,10 +6402,10 @@
         <f t="shared" si="10"/>
         <v>13.700167692307691</v>
       </c>
-      <c r="K57" s="73" t="s">
+      <c r="K57" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="L57" s="74"/>
+      <c r="L57" s="73"/>
       <c r="N57" s="9"/>
       <c r="O57" s="28" t="s">
         <v>0</v>
@@ -6362,10 +6415,10 @@
       </c>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="58" t="s">
+      <c r="B58" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="58"/>
+      <c r="C58" s="57"/>
       <c r="D58" s="51">
         <f t="array" ref="D58">_xlfn.STDEV.P(IF(D5:D55 &lt;30, D5:D55))</f>
         <v>5.6226015662019622</v>
@@ -6390,11 +6443,11 @@
         <f t="array" ref="I58">_xlfn.STDEV.P(IF(I5:I55 &lt;30, I5:I55))</f>
         <v>4.4629997383532842</v>
       </c>
-      <c r="K58" s="76" t="str">
+      <c r="K58" s="75" t="str">
         <f>+_xlfn.CONCAT(COUNTIF(K5:K55, "&lt;12.5"), "/", COUNT(K5:K55))</f>
         <v>14/51</v>
       </c>
-      <c r="L58" s="76"/>
+      <c r="L58" s="75"/>
       <c r="N58" s="27" t="s">
         <v>2</v>
       </c>
@@ -6408,10 +6461,10 @@
       </c>
     </row>
     <row r="59" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B59" s="75" t="s">
+      <c r="B59" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="75"/>
+      <c r="C59" s="74"/>
       <c r="D59" s="51" t="str">
         <f t="shared" ref="D59:I59" si="11">+_xlfn.CONCAT(COUNTIF(D5:D55, "&gt;"&amp;$U$3), "/", COUNT(D5:D55))</f>
         <v>15/51</v>
@@ -6450,8 +6503,8 @@
       </c>
     </row>
     <row r="60" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B60" s="63"/>
-      <c r="C60" s="63"/>
+      <c r="B60" s="62"/>
+      <c r="C60" s="62"/>
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
@@ -6480,11 +6533,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="B5:B55"/>
-    <mergeCell ref="B57:C57"/>
     <mergeCell ref="K57:L57"/>
     <mergeCell ref="R4:T4"/>
     <mergeCell ref="R3:T3"/>
@@ -6493,6 +6541,11 @@
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B5:B55"/>
+    <mergeCell ref="B57:C57"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:I56">
     <cfRule type="cellIs" dxfId="19" priority="7" operator="greaterThan">
@@ -6535,8 +6588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C772672-3FFA-4573-AD49-CC6DB9123722}">
   <dimension ref="B1:Q68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6557,30 +6610,30 @@
     <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11"/>
       <c r="C2" s="13"/>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="79"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="78"/>
     </row>
     <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
       <c r="C3" s="14"/>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="65"/>
-      <c r="K3" s="70" t="s">
+      <c r="E3" s="62"/>
+      <c r="F3" s="64"/>
+      <c r="K3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="72"/>
+      <c r="L3" s="71"/>
       <c r="M3" s="30"/>
-      <c r="N3" s="66" t="s">
+      <c r="N3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
       <c r="Q3" s="35">
         <v>20</v>
       </c>
@@ -6610,17 +6663,17 @@
         <v>11</v>
       </c>
       <c r="M4" s="25"/>
-      <c r="N4" s="66" t="s">
+      <c r="N4" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
       <c r="Q4" s="35">
         <v>12.5</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="67" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="14">
@@ -6654,7 +6707,7 @@
       <c r="M5" s="20"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="14">
         <v>8</v>
       </c>
@@ -6686,7 +6739,7 @@
       <c r="M6" s="20"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="68"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14">
         <v>10</v>
       </c>
@@ -6718,7 +6771,7 @@
       <c r="M7" s="20"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="68"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="14">
         <v>11</v>
       </c>
@@ -6750,7 +6803,7 @@
       <c r="M8" s="20"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="68"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="14">
         <v>13</v>
       </c>
@@ -6782,7 +6835,7 @@
       <c r="M9" s="20"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="68"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="14">
         <v>20</v>
       </c>
@@ -6814,7 +6867,7 @@
       <c r="M10" s="20"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="68"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="14">
         <v>21</v>
       </c>
@@ -6846,7 +6899,7 @@
       <c r="M11" s="20"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="68"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="14">
         <v>22</v>
       </c>
@@ -6878,7 +6931,7 @@
       <c r="M12" s="20"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="68"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="14">
         <v>23</v>
       </c>
@@ -6910,7 +6963,7 @@
       <c r="M13" s="20"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="68"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="14">
         <v>25</v>
       </c>
@@ -6942,7 +6995,7 @@
       <c r="M14" s="20"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="68"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="14">
         <v>26</v>
       </c>
@@ -6974,7 +7027,7 @@
       <c r="M15" s="20"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="68"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="14">
         <v>28</v>
       </c>
@@ -7006,7 +7059,7 @@
       <c r="M16" s="20"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="68"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="14">
         <v>30</v>
       </c>
@@ -7038,7 +7091,7 @@
       <c r="M17" s="20"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="68"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="14">
         <v>34</v>
       </c>
@@ -7070,7 +7123,7 @@
       <c r="M18" s="20"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="68"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="14">
         <v>36</v>
       </c>
@@ -7102,7 +7155,7 @@
       <c r="M19" s="20"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="68"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="14">
         <v>37</v>
       </c>
@@ -7134,7 +7187,7 @@
       <c r="M20" s="20"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="68"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="14">
         <v>40</v>
       </c>
@@ -7166,7 +7219,7 @@
       <c r="M21" s="20"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="68"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="14">
         <v>41</v>
       </c>
@@ -7198,7 +7251,7 @@
       <c r="M22" s="20"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="68"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="14">
         <v>46</v>
       </c>
@@ -7230,7 +7283,7 @@
       <c r="M23" s="20"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="68"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="14">
         <v>49</v>
       </c>
@@ -7262,7 +7315,7 @@
       <c r="M24" s="20"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="68"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="14">
         <v>50</v>
       </c>
@@ -7294,7 +7347,7 @@
       <c r="M25" s="20"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="68"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="14">
         <v>55</v>
       </c>
@@ -7326,7 +7379,7 @@
       <c r="M26" s="20"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="68"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="14">
         <v>56</v>
       </c>
@@ -7358,7 +7411,7 @@
       <c r="M27" s="20"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="68"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="14">
         <v>62</v>
       </c>
@@ -7390,7 +7443,7 @@
       <c r="M28" s="20"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="68"/>
+      <c r="B29" s="67"/>
       <c r="C29" s="14">
         <v>66</v>
       </c>
@@ -7422,7 +7475,7 @@
       <c r="M29" s="20"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="68"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="14">
         <v>67</v>
       </c>
@@ -7454,7 +7507,7 @@
       <c r="M30" s="20"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="68"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="14">
         <v>69</v>
       </c>
@@ -7486,7 +7539,7 @@
       <c r="M31" s="20"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="68"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="14">
         <v>70</v>
       </c>
@@ -7518,7 +7571,7 @@
       <c r="M32" s="20"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="68"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="14">
         <v>71</v>
       </c>
@@ -7550,7 +7603,7 @@
       <c r="M33" s="20"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="14">
         <v>74</v>
       </c>
@@ -7582,7 +7635,7 @@
       <c r="M34" s="20"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="68"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="14">
         <v>75</v>
       </c>
@@ -7614,7 +7667,7 @@
       <c r="M35" s="20"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="68"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="14">
         <v>78</v>
       </c>
@@ -7646,7 +7699,7 @@
       <c r="M36" s="20"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="68"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="14">
         <v>79</v>
       </c>
@@ -7678,7 +7731,7 @@
       <c r="M37" s="20"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="68"/>
+      <c r="B38" s="67"/>
       <c r="C38" s="14">
         <v>80</v>
       </c>
@@ -7710,7 +7763,7 @@
       <c r="M38" s="20"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="68"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="14">
         <v>81</v>
       </c>
@@ -7742,7 +7795,7 @@
       <c r="M39" s="20"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="68"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="14">
         <v>82</v>
       </c>
@@ -7774,7 +7827,7 @@
       <c r="M40" s="20"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="68"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="14">
         <v>83</v>
       </c>
@@ -7806,7 +7859,7 @@
       <c r="M41" s="20"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="68"/>
+      <c r="B42" s="67"/>
       <c r="C42" s="14">
         <v>86</v>
       </c>
@@ -7838,7 +7891,7 @@
       <c r="M42" s="20"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="68"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="14">
         <v>88</v>
       </c>
@@ -7870,7 +7923,7 @@
       <c r="M43" s="20"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="68"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="14">
         <v>90</v>
       </c>
@@ -7902,7 +7955,7 @@
       <c r="M44" s="20"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="68"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="14">
         <v>91</v>
       </c>
@@ -7934,7 +7987,7 @@
       <c r="M45" s="20"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="68"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="14">
         <v>92</v>
       </c>
@@ -7966,7 +8019,7 @@
       <c r="M46" s="20"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="68"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="14">
         <v>93</v>
       </c>
@@ -7998,7 +8051,7 @@
       <c r="M47" s="20"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="68"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="14">
         <v>94</v>
       </c>
@@ -8030,7 +8083,7 @@
       <c r="M48" s="20"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="68"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="14">
         <v>95</v>
       </c>
@@ -8062,7 +8115,7 @@
       <c r="M49" s="20"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B50" s="68"/>
+      <c r="B50" s="67"/>
       <c r="C50" s="14">
         <v>96</v>
       </c>
@@ -8094,7 +8147,7 @@
       <c r="M50" s="20"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B51" s="68"/>
+      <c r="B51" s="67"/>
       <c r="C51" s="14">
         <v>97</v>
       </c>
@@ -8126,7 +8179,7 @@
       <c r="M51" s="20"/>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="68"/>
+      <c r="B52" s="67"/>
       <c r="C52" s="14">
         <v>98</v>
       </c>
@@ -8158,7 +8211,7 @@
       <c r="M52" s="20"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="68"/>
+      <c r="B53" s="67"/>
       <c r="C53" s="14">
         <v>99</v>
       </c>
@@ -8190,7 +8243,7 @@
       <c r="M53" s="20"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B54" s="68"/>
+      <c r="B54" s="67"/>
       <c r="C54" s="14">
         <v>100</v>
       </c>
@@ -8222,7 +8275,7 @@
       <c r="M54" s="20"/>
     </row>
     <row r="55" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="69"/>
+      <c r="B55" s="68"/>
       <c r="C55" s="15">
         <v>103</v>
       </c>
@@ -8267,10 +8320,10 @@
       <c r="N56"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="58" t="s">
+      <c r="B57" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="58"/>
+      <c r="C57" s="57"/>
       <c r="D57" s="51">
         <f>+AVERAGEIF(D5:D55, "&lt;"&amp;$Q$3)</f>
         <v>13.797277500000002</v>
@@ -8283,10 +8336,10 @@
         <f>+AVERAGEIF(F5:F55, "&lt;"&amp;$Q$3)</f>
         <v>14.19857722222222</v>
       </c>
-      <c r="H57" s="58" t="s">
+      <c r="H57" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="I57" s="58"/>
+      <c r="I57" s="57"/>
       <c r="L57" s="28" t="s">
         <v>11</v>
       </c>
@@ -8294,10 +8347,10 @@
       <c r="N57"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="58" t="s">
+      <c r="B58" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="58"/>
+      <c r="C58" s="57"/>
       <c r="D58" s="51">
         <f t="array" ref="D58">_xlfn.STDEV.P(IF(D5:D55 &lt;30, D5:D55))</f>
         <v>5.2425968161030445</v>
@@ -8310,11 +8363,11 @@
         <f t="array" ref="F58">_xlfn.STDEV.P(IF(F5:F55 &lt;30, F5:F55))</f>
         <v>5.2798524809432124</v>
       </c>
-      <c r="H58" s="76" t="str">
+      <c r="H58" s="75" t="str">
         <f>+_xlfn.CONCAT(COUNTIF(H5:H55, "&lt;"&amp;$Q$4), "/", COUNT(H5:H55))</f>
         <v>17/51</v>
       </c>
-      <c r="I58" s="76"/>
+      <c r="I58" s="75"/>
       <c r="K58" s="27" t="s">
         <v>2</v>
       </c>
@@ -8326,10 +8379,10 @@
       <c r="N58"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="75" t="s">
+      <c r="B59" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="75"/>
+      <c r="C59" s="74"/>
       <c r="D59" s="29" t="str">
         <f>+_xlfn.CONCAT(COUNTIF(D5:D55, "&gt;"&amp;$Q$3), "/", COUNT(D5:D55))</f>
         <v>15/51</v>
@@ -8385,17 +8438,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="B5:B55"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="H57:I57"/>
     <mergeCell ref="H58:I58"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B5:B55"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:F56">
     <cfRule type="cellIs" dxfId="12" priority="6" operator="greaterThan">
@@ -8432,8 +8485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264EAE38-2C34-416B-82D7-BB0AE0C984BB}">
   <dimension ref="B1:U68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8456,30 +8509,30 @@
     <row r="2" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11"/>
       <c r="C2" s="13"/>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="79"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="78"/>
     </row>
     <row r="3" spans="2:21" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
       <c r="C3" s="14"/>
-      <c r="D3" s="80" t="s">
+      <c r="D3" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="81"/>
-      <c r="F3" s="82"/>
-      <c r="K3" s="70" t="s">
+      <c r="E3" s="80"/>
+      <c r="F3" s="81"/>
+      <c r="K3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="72"/>
+      <c r="L3" s="71"/>
       <c r="M3" s="30"/>
-      <c r="N3" s="66" t="s">
+      <c r="N3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
       <c r="Q3" s="50">
         <v>20</v>
       </c>
@@ -8509,18 +8562,18 @@
         <v>11</v>
       </c>
       <c r="M4" s="34"/>
-      <c r="N4" s="66" t="s">
+      <c r="N4" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
       <c r="Q4" s="50">
         <v>12.5</v>
       </c>
-      <c r="U4" s="55"/>
+      <c r="U4" s="54"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="67" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="14">
@@ -8552,10 +8605,10 @@
         <v>NCC</v>
       </c>
       <c r="M5" s="48"/>
-      <c r="U5" s="55"/>
+      <c r="U5" s="54"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="14">
         <v>8</v>
       </c>
@@ -8585,10 +8638,10 @@
         <v>MI</v>
       </c>
       <c r="M6" s="48"/>
-      <c r="U6" s="55"/>
+      <c r="U6" s="54"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="68"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14">
         <v>10</v>
       </c>
@@ -8618,10 +8671,10 @@
         <v>NCC</v>
       </c>
       <c r="M7" s="48"/>
-      <c r="U7" s="55"/>
+      <c r="U7" s="54"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="68"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="14">
         <v>11</v>
       </c>
@@ -8651,10 +8704,10 @@
         <v>SSD</v>
       </c>
       <c r="M8" s="48"/>
-      <c r="U8" s="55"/>
+      <c r="U8" s="54"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="68"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="14">
         <v>13</v>
       </c>
@@ -8684,10 +8737,10 @@
         <v>NCC</v>
       </c>
       <c r="M9" s="48"/>
-      <c r="U9" s="55"/>
+      <c r="U9" s="54"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="68"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="14">
         <v>20</v>
       </c>
@@ -8717,10 +8770,10 @@
         <v>NCC</v>
       </c>
       <c r="M10" s="48"/>
-      <c r="U10" s="55"/>
+      <c r="U10" s="54"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="68"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="14">
         <v>21</v>
       </c>
@@ -8750,10 +8803,10 @@
         <v>NCC</v>
       </c>
       <c r="M11" s="48"/>
-      <c r="U11" s="55"/>
+      <c r="U11" s="54"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="68"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="14">
         <v>22</v>
       </c>
@@ -8783,10 +8836,10 @@
         <v>NCC</v>
       </c>
       <c r="M12" s="48"/>
-      <c r="U12" s="55"/>
+      <c r="U12" s="54"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="68"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="14">
         <v>23</v>
       </c>
@@ -8816,10 +8869,10 @@
         <v>NCC</v>
       </c>
       <c r="M13" s="48"/>
-      <c r="U13" s="55"/>
+      <c r="U13" s="54"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="68"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="14">
         <v>25</v>
       </c>
@@ -8849,10 +8902,10 @@
         <v>MI</v>
       </c>
       <c r="M14" s="48"/>
-      <c r="U14" s="55"/>
+      <c r="U14" s="54"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="68"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="14">
         <v>26</v>
       </c>
@@ -8882,10 +8935,10 @@
         <v>NCC</v>
       </c>
       <c r="M15" s="48"/>
-      <c r="U15" s="55"/>
+      <c r="U15" s="54"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="68"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="14">
         <v>28</v>
       </c>
@@ -8915,10 +8968,10 @@
         <v>NCC</v>
       </c>
       <c r="M16" s="48"/>
-      <c r="U16" s="55"/>
+      <c r="U16" s="54"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="68"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="14">
         <v>30</v>
       </c>
@@ -8948,10 +9001,10 @@
         <v>NCC</v>
       </c>
       <c r="M17" s="48"/>
-      <c r="U17" s="55"/>
+      <c r="U17" s="54"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="68"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="14">
         <v>34</v>
       </c>
@@ -8981,10 +9034,10 @@
         <v>SSD</v>
       </c>
       <c r="M18" s="48"/>
-      <c r="U18" s="55"/>
+      <c r="U18" s="54"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="68"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="14">
         <v>36</v>
       </c>
@@ -9014,10 +9067,10 @@
         <v>NCC</v>
       </c>
       <c r="M19" s="48"/>
-      <c r="U19" s="55"/>
+      <c r="U19" s="54"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="68"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="14">
         <v>37</v>
       </c>
@@ -9047,10 +9100,10 @@
         <v>NCC</v>
       </c>
       <c r="M20" s="48"/>
-      <c r="U20" s="55"/>
+      <c r="U20" s="54"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="68"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="14">
         <v>40</v>
       </c>
@@ -9080,10 +9133,10 @@
         <v>SSD</v>
       </c>
       <c r="M21" s="48"/>
-      <c r="U21" s="55"/>
+      <c r="U21" s="54"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="68"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="14">
         <v>41</v>
       </c>
@@ -9113,10 +9166,10 @@
         <v>NCC</v>
       </c>
       <c r="M22" s="48"/>
-      <c r="U22" s="55"/>
+      <c r="U22" s="54"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B23" s="68"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="14">
         <v>46</v>
       </c>
@@ -9146,10 +9199,10 @@
         <v>NCC</v>
       </c>
       <c r="M23" s="48"/>
-      <c r="U23" s="55"/>
+      <c r="U23" s="54"/>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B24" s="68"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="14">
         <v>49</v>
       </c>
@@ -9179,10 +9232,10 @@
         <v>NCC</v>
       </c>
       <c r="M24" s="48"/>
-      <c r="U24" s="55"/>
+      <c r="U24" s="54"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="68"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="14">
         <v>50</v>
       </c>
@@ -9212,10 +9265,10 @@
         <v>SSD</v>
       </c>
       <c r="M25" s="48"/>
-      <c r="U25" s="55"/>
+      <c r="U25" s="54"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B26" s="68"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="14">
         <v>55</v>
       </c>
@@ -9245,10 +9298,10 @@
         <v>NCC</v>
       </c>
       <c r="M26" s="48"/>
-      <c r="U26" s="55"/>
+      <c r="U26" s="54"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B27" s="68"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="14">
         <v>56</v>
       </c>
@@ -9278,10 +9331,10 @@
         <v>NCC</v>
       </c>
       <c r="M27" s="48"/>
-      <c r="U27" s="55"/>
+      <c r="U27" s="54"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B28" s="68"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="14">
         <v>62</v>
       </c>
@@ -9311,10 +9364,10 @@
         <v>NCC</v>
       </c>
       <c r="M28" s="48"/>
-      <c r="U28" s="55"/>
+      <c r="U28" s="54"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="68"/>
+      <c r="B29" s="67"/>
       <c r="C29" s="14">
         <v>66</v>
       </c>
@@ -9344,10 +9397,10 @@
         <v>NCC</v>
       </c>
       <c r="M29" s="48"/>
-      <c r="U29" s="55"/>
+      <c r="U29" s="54"/>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="68"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="14">
         <v>67</v>
       </c>
@@ -9377,10 +9430,10 @@
         <v>MI</v>
       </c>
       <c r="M30" s="48"/>
-      <c r="U30" s="55"/>
+      <c r="U30" s="54"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B31" s="68"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="14">
         <v>69</v>
       </c>
@@ -9410,10 +9463,10 @@
         <v>NCC</v>
       </c>
       <c r="M31" s="48"/>
-      <c r="U31" s="55"/>
+      <c r="U31" s="54"/>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B32" s="68"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="14">
         <v>70</v>
       </c>
@@ -9443,10 +9496,10 @@
         <v>NCC</v>
       </c>
       <c r="M32" s="48"/>
-      <c r="U32" s="55"/>
+      <c r="U32" s="54"/>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B33" s="68"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="14">
         <v>71</v>
       </c>
@@ -9476,10 +9529,10 @@
         <v>NCC</v>
       </c>
       <c r="M33" s="48"/>
-      <c r="U33" s="55"/>
+      <c r="U33" s="54"/>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="14">
         <v>74</v>
       </c>
@@ -9509,10 +9562,10 @@
         <v>NCC</v>
       </c>
       <c r="M34" s="48"/>
-      <c r="U34" s="55"/>
+      <c r="U34" s="54"/>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B35" s="68"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="14">
         <v>75</v>
       </c>
@@ -9542,10 +9595,10 @@
         <v>NCC</v>
       </c>
       <c r="M35" s="48"/>
-      <c r="U35" s="55"/>
+      <c r="U35" s="54"/>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B36" s="68"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="14">
         <v>78</v>
       </c>
@@ -9575,10 +9628,10 @@
         <v>NCC</v>
       </c>
       <c r="M36" s="48"/>
-      <c r="U36" s="55"/>
+      <c r="U36" s="54"/>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B37" s="68"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="14">
         <v>79</v>
       </c>
@@ -9608,10 +9661,10 @@
         <v>NCC</v>
       </c>
       <c r="M37" s="48"/>
-      <c r="U37" s="55"/>
+      <c r="U37" s="54"/>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B38" s="68"/>
+      <c r="B38" s="67"/>
       <c r="C38" s="14">
         <v>80</v>
       </c>
@@ -9641,10 +9694,10 @@
         <v>NCC</v>
       </c>
       <c r="M38" s="48"/>
-      <c r="U38" s="55"/>
+      <c r="U38" s="54"/>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B39" s="68"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="14">
         <v>81</v>
       </c>
@@ -9674,10 +9727,10 @@
         <v>SSD</v>
       </c>
       <c r="M39" s="48"/>
-      <c r="U39" s="55"/>
+      <c r="U39" s="54"/>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B40" s="68"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="14">
         <v>82</v>
       </c>
@@ -9707,10 +9760,10 @@
         <v>NCC</v>
       </c>
       <c r="M40" s="48"/>
-      <c r="U40" s="55"/>
+      <c r="U40" s="54"/>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B41" s="68"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="14">
         <v>83</v>
       </c>
@@ -9740,10 +9793,10 @@
         <v>NCC</v>
       </c>
       <c r="M41" s="48"/>
-      <c r="U41" s="55"/>
+      <c r="U41" s="54"/>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B42" s="68"/>
+      <c r="B42" s="67"/>
       <c r="C42" s="14">
         <v>86</v>
       </c>
@@ -9773,10 +9826,10 @@
         <v>NCC</v>
       </c>
       <c r="M42" s="48"/>
-      <c r="U42" s="55"/>
+      <c r="U42" s="54"/>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B43" s="68"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="14">
         <v>88</v>
       </c>
@@ -9806,10 +9859,10 @@
         <v>NCC</v>
       </c>
       <c r="M43" s="48"/>
-      <c r="U43" s="55"/>
+      <c r="U43" s="54"/>
     </row>
     <row r="44" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B44" s="68"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="14">
         <v>90</v>
       </c>
@@ -9839,10 +9892,10 @@
         <v>SSD</v>
       </c>
       <c r="M44" s="48"/>
-      <c r="U44" s="55"/>
+      <c r="U44" s="54"/>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B45" s="68"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="14">
         <v>91</v>
       </c>
@@ -9872,10 +9925,10 @@
         <v>NCC</v>
       </c>
       <c r="M45" s="48"/>
-      <c r="U45" s="55"/>
+      <c r="U45" s="54"/>
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B46" s="68"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="14">
         <v>92</v>
       </c>
@@ -9905,10 +9958,10 @@
         <v>NCC</v>
       </c>
       <c r="M46" s="48"/>
-      <c r="U46" s="55"/>
+      <c r="U46" s="54"/>
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B47" s="68"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="14">
         <v>93</v>
       </c>
@@ -9938,10 +9991,10 @@
         <v>NCC</v>
       </c>
       <c r="M47" s="48"/>
-      <c r="U47" s="55"/>
+      <c r="U47" s="54"/>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B48" s="68"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="14">
         <v>94</v>
       </c>
@@ -9971,10 +10024,10 @@
         <v>MI</v>
       </c>
       <c r="M48" s="48"/>
-      <c r="U48" s="55"/>
+      <c r="U48" s="54"/>
     </row>
     <row r="49" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B49" s="68"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="14">
         <v>95</v>
       </c>
@@ -10004,10 +10057,10 @@
         <v>NCC</v>
       </c>
       <c r="M49" s="48"/>
-      <c r="U49" s="55"/>
+      <c r="U49" s="54"/>
     </row>
     <row r="50" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B50" s="68"/>
+      <c r="B50" s="67"/>
       <c r="C50" s="14">
         <v>96</v>
       </c>
@@ -10037,10 +10090,10 @@
         <v>NCC</v>
       </c>
       <c r="M50" s="48"/>
-      <c r="U50" s="55"/>
+      <c r="U50" s="54"/>
     </row>
     <row r="51" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B51" s="68"/>
+      <c r="B51" s="67"/>
       <c r="C51" s="14">
         <v>97</v>
       </c>
@@ -10070,10 +10123,10 @@
         <v>NCC</v>
       </c>
       <c r="M51" s="48"/>
-      <c r="U51" s="55"/>
+      <c r="U51" s="54"/>
     </row>
     <row r="52" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B52" s="68"/>
+      <c r="B52" s="67"/>
       <c r="C52" s="14">
         <v>98</v>
       </c>
@@ -10103,10 +10156,10 @@
         <v>MI</v>
       </c>
       <c r="M52" s="48"/>
-      <c r="U52" s="55"/>
+      <c r="U52" s="54"/>
     </row>
     <row r="53" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B53" s="68"/>
+      <c r="B53" s="67"/>
       <c r="C53" s="14">
         <v>99</v>
       </c>
@@ -10136,10 +10189,10 @@
         <v>MI</v>
       </c>
       <c r="M53" s="48"/>
-      <c r="U53" s="55"/>
+      <c r="U53" s="54"/>
     </row>
     <row r="54" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B54" s="68"/>
+      <c r="B54" s="67"/>
       <c r="C54" s="14">
         <v>100</v>
       </c>
@@ -10169,10 +10222,10 @@
         <v>NCC</v>
       </c>
       <c r="M54" s="48"/>
-      <c r="U54" s="55"/>
+      <c r="U54" s="54"/>
     </row>
     <row r="55" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="69"/>
+      <c r="B55" s="68"/>
       <c r="C55" s="15">
         <v>103</v>
       </c>
@@ -10217,7 +10270,7 @@
       <c r="N56"/>
     </row>
     <row r="57" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C57" s="53" t="s">
+      <c r="C57" s="52" t="s">
         <v>8</v>
       </c>
       <c r="D57" s="51">
@@ -10232,10 +10285,10 @@
         <f>+AVERAGEIF(F5:F55, "&lt;"&amp;$Q$3)</f>
         <v>14.704215128205131</v>
       </c>
-      <c r="H57" s="58" t="s">
+      <c r="H57" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="I57" s="58"/>
+      <c r="I57" s="57"/>
       <c r="L57" s="28" t="s">
         <v>11</v>
       </c>
@@ -10243,7 +10296,7 @@
       <c r="N57"/>
     </row>
     <row r="58" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C58" s="53" t="s">
+      <c r="C58" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="51">
@@ -10258,11 +10311,11 @@
         <f t="array" ref="F58">_xlfn.STDEV.P(IF(F5:F55 &lt;30, F5:F55))</f>
         <v>4.3985422286912064</v>
       </c>
-      <c r="H58" s="76" t="str">
+      <c r="H58" s="75" t="str">
         <f>+_xlfn.CONCAT(COUNTIF(H5:H55, "&lt;"&amp;$Q$4), "/", COUNT(H5:H55))</f>
         <v>13/51</v>
       </c>
-      <c r="I58" s="76"/>
+      <c r="I58" s="75"/>
       <c r="K58" s="47" t="s">
         <v>2</v>
       </c>
@@ -10274,7 +10327,7 @@
       <c r="N58"/>
     </row>
     <row r="59" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="54" t="s">
+      <c r="C59" s="53" t="s">
         <v>10</v>
       </c>
       <c r="D59" s="51" t="str">
@@ -10332,14 +10385,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H58:I58"/>
     <mergeCell ref="B5:B55"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="N4:P4"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H58:I58"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:F56">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
@@ -10379,877 +10432,812 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A4E032-52BD-4D58-892B-7752E582F2AC}">
-  <dimension ref="D4:F146"/>
+  <dimension ref="B2:I147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="36"/>
+    <col min="2" max="2" width="9.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="36" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="36"/>
+    <col min="7" max="7" width="7.85546875" style="36" customWidth="1"/>
+    <col min="8" max="9" width="7.7109375" style="36" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="36"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="52">
-        <f>+'sirt-deformable-reg'!E5 - 'sirt-linear-deformable-reg'!E5</f>
-        <v>-0.89300000000000068</v>
-      </c>
-    </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="52">
-        <f>+'sirt-deformable-reg'!E6 - 'sirt-linear-deformable-reg'!E6</f>
-        <v>-5.1952999999999978</v>
-      </c>
-    </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="52">
-        <f>+'sirt-deformable-reg'!E7 - 'sirt-linear-deformable-reg'!E7</f>
-        <v>-1.4579999999999984</v>
-      </c>
-      <c r="F6">
-        <f>+COUNTIF(D4:D56, "&gt;0")</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="52">
-        <f>+'sirt-deformable-reg'!E8 - 'sirt-linear-deformable-reg'!E8</f>
-        <v>-0.16109999999999935</v>
-      </c>
-    </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="52">
-        <f>+'sirt-deformable-reg'!E9 - 'sirt-linear-deformable-reg'!E9</f>
-        <v>-1.3585999999999991</v>
-      </c>
-    </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="52">
-        <f>+'sirt-deformable-reg'!E10 - 'sirt-linear-deformable-reg'!E10</f>
-        <v>-1.8390000000000022</v>
-      </c>
-    </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="52">
-        <f>+'sirt-deformable-reg'!E11 - 'sirt-linear-deformable-reg'!E11</f>
-        <v>-1.4860000000000007</v>
-      </c>
-    </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="52">
-        <f>+'sirt-deformable-reg'!E12 - 'sirt-linear-deformable-reg'!E12</f>
-        <v>-0.11359999999999992</v>
-      </c>
-    </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="52">
-        <f>+'sirt-deformable-reg'!E13 - 'sirt-linear-deformable-reg'!E13</f>
-        <v>-2.7498000000000005</v>
-      </c>
-    </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="52">
-        <f>+'sirt-deformable-reg'!E14 - 'sirt-linear-deformable-reg'!E14</f>
-        <v>-1.3535000000000004</v>
-      </c>
-    </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="52">
-        <f>+'sirt-deformable-reg'!E15 - 'sirt-linear-deformable-reg'!E15</f>
-        <v>-2.3902999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="52">
-        <f>+'sirt-deformable-reg'!E16 - 'sirt-linear-deformable-reg'!E16</f>
-        <v>-4.8501000000000012</v>
-      </c>
-    </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="52">
-        <f>+'sirt-deformable-reg'!E17 - 'sirt-linear-deformable-reg'!E17</f>
-        <v>-3.8511000000000006</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="52">
-        <f>+'sirt-deformable-reg'!E18 - 'sirt-linear-deformable-reg'!E18</f>
-        <v>-3.4890000000000043</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="52">
-        <f>+'sirt-deformable-reg'!E19 - 'sirt-linear-deformable-reg'!E19</f>
-        <v>-2.0597000000000012</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="52">
-        <f>+'sirt-deformable-reg'!E20 - 'sirt-linear-deformable-reg'!E20</f>
-        <v>-5.2908999999999988</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="52">
-        <f>+'sirt-deformable-reg'!E21 - 'sirt-linear-deformable-reg'!E21</f>
-        <v>-0.48880000000000123</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D21" s="52">
-        <f>+'sirt-deformable-reg'!E22 - 'sirt-linear-deformable-reg'!E22</f>
-        <v>-0.1041799999999995</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="52">
-        <f>+'sirt-deformable-reg'!E23 - 'sirt-linear-deformable-reg'!E23</f>
-        <v>-1.8889300000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="52">
-        <f>+'sirt-deformable-reg'!E24 - 'sirt-linear-deformable-reg'!E24</f>
-        <v>1.4579000000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="52">
-        <f>+'sirt-deformable-reg'!E25 - 'sirt-linear-deformable-reg'!E25</f>
-        <v>-1.7839999999999989</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="52">
-        <f>+'sirt-deformable-reg'!E26 - 'sirt-linear-deformable-reg'!E26</f>
-        <v>-2.1506000000000007</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="52">
-        <f>+'sirt-deformable-reg'!E27 - 'sirt-linear-deformable-reg'!E27</f>
-        <v>-1.0730000000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D27" s="52">
-        <f>+'sirt-deformable-reg'!E28 - 'sirt-linear-deformable-reg'!E28</f>
-        <v>-1.6524599999999996</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="52">
-        <f>+'sirt-deformable-reg'!E29 - 'sirt-linear-deformable-reg'!E29</f>
-        <v>-2.0833000000000013</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="52">
-        <f>+'sirt-deformable-reg'!E30 - 'sirt-linear-deformable-reg'!E30</f>
-        <v>-2.0419000000000018</v>
-      </c>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="52">
-        <f>+'sirt-deformable-reg'!E31 - 'sirt-linear-deformable-reg'!E31</f>
-        <v>0.56159999999999854</v>
-      </c>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D31" s="52">
-        <f>+'sirt-deformable-reg'!E32 - 'sirt-linear-deformable-reg'!E32</f>
-        <v>-1.0897600000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D32" s="52">
-        <f>+'sirt-deformable-reg'!E33 - 'sirt-linear-deformable-reg'!E33</f>
-        <v>2.0520999999999994</v>
-      </c>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="88" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="G3" s="89" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="89"/>
+      <c r="C4" s="90">
+        <v>333</v>
+      </c>
+      <c r="D4" s="90">
+        <v>444</v>
+      </c>
+      <c r="E4" s="90">
+        <v>555</v>
+      </c>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="82">
+        <v>25</v>
+      </c>
+      <c r="C5" s="83">
+        <v>11.176299999999999</v>
+      </c>
+      <c r="D5" s="83">
+        <v>11.12</v>
+      </c>
+      <c r="E5" s="83">
+        <v>11.282999999999999</v>
+      </c>
+      <c r="G5" s="36">
+        <v>75</v>
+      </c>
+      <c r="H5" s="36">
+        <v>322</v>
+      </c>
+      <c r="I5" s="36">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="82">
+        <v>41</v>
+      </c>
+      <c r="C6" s="83">
+        <v>10.4496</v>
+      </c>
+      <c r="D6" s="83">
+        <v>9.1877200000000006</v>
+      </c>
+      <c r="E6" s="83">
+        <v>9.86205</v>
+      </c>
+      <c r="G6" s="36">
+        <v>17</v>
+      </c>
+      <c r="H6" s="36">
+        <v>154</v>
+      </c>
+      <c r="I6" s="36">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="82">
+        <v>46</v>
+      </c>
+      <c r="C7" s="83">
+        <v>10.575200000000001</v>
+      </c>
+      <c r="D7" s="83">
+        <v>9.7514699999999994</v>
+      </c>
+      <c r="E7" s="83">
+        <v>9.3211700000000004</v>
+      </c>
+      <c r="G7" s="36">
+        <v>99</v>
+      </c>
+      <c r="H7" s="36">
+        <v>184</v>
+      </c>
+      <c r="I7" s="36">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="82">
+        <v>55</v>
+      </c>
+      <c r="C8" s="83">
+        <v>13.5726</v>
+      </c>
+      <c r="D8" s="83">
+        <v>10.3111</v>
+      </c>
+      <c r="E8" s="83">
+        <v>10.6937</v>
+      </c>
+      <c r="G8" s="36">
+        <v>17</v>
+      </c>
+      <c r="H8" s="36">
+        <v>136</v>
+      </c>
+      <c r="I8" s="36">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="82">
+        <v>62</v>
+      </c>
+      <c r="C9" s="83">
+        <v>10.238200000000001</v>
+      </c>
+      <c r="D9" s="83">
+        <v>9.39574</v>
+      </c>
+      <c r="E9" s="83">
+        <v>10.064299999999999</v>
+      </c>
+      <c r="G9" s="36">
+        <v>80</v>
+      </c>
+      <c r="H9" s="36">
+        <v>290</v>
+      </c>
+      <c r="I9" s="36">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="82">
+        <v>70</v>
+      </c>
+      <c r="C10" s="83">
+        <v>8.3791399999999996</v>
+      </c>
+      <c r="D10" s="83">
+        <v>8.2635299999999994</v>
+      </c>
+      <c r="E10" s="83">
+        <v>7.6331300000000004</v>
+      </c>
+      <c r="G10" s="36">
+        <v>22</v>
+      </c>
+      <c r="H10" s="36">
+        <v>53</v>
+      </c>
+      <c r="I10" s="36">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="82">
+        <v>80</v>
+      </c>
+      <c r="C11" s="83">
+        <v>8.7020999999999997</v>
+      </c>
+      <c r="D11" s="83">
+        <v>8.5310000000000006</v>
+      </c>
+      <c r="E11" s="83">
+        <v>8.2985500000000005</v>
+      </c>
+      <c r="G11" s="36">
+        <v>42</v>
+      </c>
+      <c r="H11" s="36">
+        <v>194</v>
+      </c>
+      <c r="I11" s="36">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="82">
+        <v>86</v>
+      </c>
+      <c r="C12" s="83">
+        <v>12.162800000000001</v>
+      </c>
+      <c r="D12" s="83">
+        <v>10.66</v>
+      </c>
+      <c r="E12" s="83">
+        <v>10.4274</v>
+      </c>
+      <c r="G12" s="36">
+        <v>15</v>
+      </c>
+      <c r="H12" s="36">
+        <v>160</v>
+      </c>
+      <c r="I12" s="36">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="82">
+        <v>93</v>
+      </c>
+      <c r="C13" s="83">
+        <v>11.1435</v>
+      </c>
+      <c r="D13" s="83">
+        <v>8.3450000000000006</v>
+      </c>
+      <c r="E13" s="83">
+        <v>8.3947099999999999</v>
+      </c>
+      <c r="G13" s="36">
+        <v>18</v>
+      </c>
+      <c r="H13" s="36">
+        <v>201</v>
+      </c>
+      <c r="I13" s="36">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="82">
+        <v>94</v>
+      </c>
+      <c r="C14" s="83">
+        <v>6.2317999999999998</v>
+      </c>
+      <c r="D14" s="83">
+        <v>6.3259100000000004</v>
+      </c>
+      <c r="E14" s="83">
+        <v>6.1532900000000001</v>
+      </c>
+      <c r="G14" s="36">
+        <v>16</v>
+      </c>
+      <c r="H14" s="36">
+        <v>45</v>
+      </c>
+      <c r="I14" s="36">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="82">
+        <v>96</v>
+      </c>
+      <c r="C15" s="83">
+        <v>12.368600000000001</v>
+      </c>
+      <c r="D15" s="83">
+        <v>9.8608799999999999</v>
+      </c>
+      <c r="E15" s="83">
+        <v>12.0588</v>
+      </c>
+      <c r="G15" s="36">
+        <v>18</v>
+      </c>
+      <c r="H15" s="36">
+        <v>171</v>
+      </c>
+      <c r="I15" s="36">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="82">
+        <v>98</v>
+      </c>
+      <c r="C16" s="83">
+        <v>11.8965</v>
+      </c>
+      <c r="D16" s="83">
+        <v>11.7354</v>
+      </c>
+      <c r="E16" s="83">
+        <v>11.3833</v>
+      </c>
+      <c r="G16" s="36">
+        <v>68</v>
+      </c>
+      <c r="H16" s="36">
+        <v>167</v>
+      </c>
+      <c r="I16" s="36">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="82">
+        <v>103</v>
+      </c>
+      <c r="C17" s="83">
+        <v>15.206</v>
+      </c>
+      <c r="D17" s="83">
+        <v>9.9429400000000001</v>
+      </c>
+      <c r="E17" s="83">
+        <v>11.181100000000001</v>
+      </c>
+      <c r="G17" s="36">
+        <v>17</v>
+      </c>
+      <c r="H17" s="36">
+        <v>193</v>
+      </c>
+      <c r="I17" s="36">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="87" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="86">
+        <f>AVERAGE(C5:C17)</f>
+        <v>10.930949230769233</v>
+      </c>
+      <c r="D18" s="86">
+        <f>AVERAGE(D5:D17)</f>
+        <v>9.4946684615384616</v>
+      </c>
+      <c r="E18" s="86">
+        <f>AVERAGE(E5:E17)</f>
+        <v>9.7503461538461558</v>
+      </c>
+      <c r="G18" s="86">
+        <f>AVERAGE(G5:G17)</f>
+        <v>38.769230769230766</v>
+      </c>
+      <c r="H18" s="86">
+        <f t="shared" ref="H18:I18" si="0">AVERAGE(H5:H17)</f>
+        <v>174.61538461538461</v>
+      </c>
+      <c r="I18" s="86">
+        <f t="shared" si="0"/>
+        <v>313.15384615384613</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="84">
+        <f>G19</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="84">
+        <f t="shared" ref="D19:E19" si="1">H19</f>
+        <v>4.503968253968254</v>
+      </c>
+      <c r="E19" s="84">
+        <f t="shared" si="1"/>
+        <v>8.0773809523809526</v>
+      </c>
+      <c r="G19" s="36">
+        <f>G18/$G$18</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="84">
+        <f>H18/$G$18</f>
+        <v>4.503968253968254</v>
+      </c>
+      <c r="I19" s="84">
+        <f>I18/$G$18</f>
+        <v>8.0773809523809526</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="85"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="85"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="85"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="85"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="85"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="85"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="85"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="85"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="85"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="85"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="85"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="85"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="85"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="52">
-        <f>+'sirt-deformable-reg'!E34 - 'sirt-linear-deformable-reg'!E34</f>
-        <v>-0.26600000000000179</v>
-      </c>
+      <c r="D33" s="85"/>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="52">
-        <f>+'sirt-deformable-reg'!E35 - 'sirt-linear-deformable-reg'!E35</f>
-        <v>-2.1510800000000003</v>
-      </c>
+      <c r="D34" s="85"/>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="52">
-        <f>+'sirt-deformable-reg'!E36 - 'sirt-linear-deformable-reg'!E36</f>
-        <v>-1.5317000000000007</v>
-      </c>
+      <c r="D35" s="85"/>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="52">
-        <f>+'sirt-deformable-reg'!E37 - 'sirt-linear-deformable-reg'!E37</f>
-        <v>0.31060000000000088</v>
-      </c>
+      <c r="D36" s="85"/>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="52">
-        <f>+'sirt-deformable-reg'!E38 - 'sirt-linear-deformable-reg'!E38</f>
-        <v>-2.2165999999999997</v>
-      </c>
+      <c r="D37" s="85"/>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="52">
-        <f>+'sirt-deformable-reg'!E39 - 'sirt-linear-deformable-reg'!E39</f>
-        <v>-0.55999999999999872</v>
-      </c>
+      <c r="D38" s="85"/>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="52">
-        <f>+'sirt-deformable-reg'!E40 - 'sirt-linear-deformable-reg'!E40</f>
-        <v>-2.0595999999999997</v>
-      </c>
+      <c r="D39" s="85"/>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="52">
-        <f>+'sirt-deformable-reg'!E41 - 'sirt-linear-deformable-reg'!E41</f>
-        <v>-5.7149999999999981</v>
-      </c>
+      <c r="D40" s="85"/>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D41" s="52">
-        <f>+'sirt-deformable-reg'!E42 - 'sirt-linear-deformable-reg'!E42</f>
-        <v>-2.3181000000000012</v>
-      </c>
+      <c r="D41" s="85"/>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D42" s="52">
-        <f>+'sirt-deformable-reg'!E43 - 'sirt-linear-deformable-reg'!E43</f>
-        <v>-6.2318999999999996</v>
-      </c>
+      <c r="D42" s="85"/>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="52">
-        <f>+'sirt-deformable-reg'!E44 - 'sirt-linear-deformable-reg'!E44</f>
-        <v>1.8383000000000003</v>
-      </c>
+      <c r="D43" s="85"/>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D44" s="52">
-        <f>+'sirt-deformable-reg'!E45 - 'sirt-linear-deformable-reg'!E45</f>
-        <v>0.24080000000000013</v>
-      </c>
+      <c r="D44" s="85"/>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D45" s="52">
-        <f>+'sirt-deformable-reg'!E46 - 'sirt-linear-deformable-reg'!E46</f>
-        <v>2.7394999999999996</v>
-      </c>
+      <c r="D45" s="85"/>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D46" s="52">
-        <f>+'sirt-deformable-reg'!E47 - 'sirt-linear-deformable-reg'!E47</f>
-        <v>-4.0688999999999993</v>
-      </c>
+      <c r="D46" s="85"/>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="52">
-        <f>+'sirt-deformable-reg'!E48 - 'sirt-linear-deformable-reg'!E48</f>
-        <v>-3.7906899999999997</v>
-      </c>
+      <c r="D47" s="85"/>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="52">
-        <f>+'sirt-deformable-reg'!E49 - 'sirt-linear-deformable-reg'!E49</f>
-        <v>-4.0552299999999999</v>
-      </c>
+      <c r="D48" s="85"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="52">
-        <f>+'sirt-deformable-reg'!E50 - 'sirt-linear-deformable-reg'!E50</f>
-        <v>1.7979199999999995</v>
-      </c>
+      <c r="D49" s="85"/>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="52">
-        <f>+'sirt-deformable-reg'!E51 - 'sirt-linear-deformable-reg'!E51</f>
-        <v>3.2284999999999986</v>
-      </c>
+      <c r="D50" s="85"/>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="52">
-        <f>+'sirt-deformable-reg'!E52 - 'sirt-linear-deformable-reg'!E52</f>
-        <v>1.6045999999999996</v>
-      </c>
+      <c r="D51" s="85"/>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="52">
-        <f>+'sirt-deformable-reg'!E53 - 'sirt-linear-deformable-reg'!E53</f>
-        <v>2.4417999999999989</v>
-      </c>
+      <c r="D52" s="85"/>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="52">
-        <f>+'sirt-deformable-reg'!E54 - 'sirt-linear-deformable-reg'!E54</f>
-        <v>-1.9718999999999998</v>
-      </c>
+      <c r="D53" s="85"/>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="52">
-        <f>+'sirt-deformable-reg'!E55 - 'sirt-linear-deformable-reg'!E55</f>
-        <v>-0.33007000000000097</v>
-      </c>
+      <c r="D54" s="85"/>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="52">
-        <f>+'sirt-deformable-reg'!E56 - 'sirt-linear-deformable-reg'!E56</f>
-        <v>0</v>
-      </c>
+      <c r="D55" s="85"/>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="52">
-        <f>+'sirt-deformable-reg'!E57 - 'sirt-linear-deformable-reg'!E57</f>
-        <v>-0.96140722619047558</v>
-      </c>
+      <c r="D56" s="85"/>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="52">
-        <f>+'sirt-deformable-reg'!E58 - 'sirt-linear-deformable-reg'!E58</f>
-        <v>0.31376204675411845</v>
-      </c>
+      <c r="D57" s="85"/>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="52">
-        <f>+'sirt-deformable-reg'!E59 - 'sirt-linear-deformable-reg'!E59</f>
-        <v>-61</v>
-      </c>
+      <c r="D58" s="85"/>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="52">
-        <f>+'sirt-deformable-reg'!E60 - 'sirt-linear-deformable-reg'!E60</f>
-        <v>0</v>
-      </c>
+      <c r="D59" s="85"/>
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="52">
-        <f>+'sirt-deformable-reg'!E61 - 'sirt-linear-deformable-reg'!E61</f>
-        <v>0</v>
-      </c>
+      <c r="D60" s="85"/>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="52">
-        <f>+'sirt-deformable-reg'!E62 - 'sirt-linear-deformable-reg'!E62</f>
-        <v>0</v>
-      </c>
+      <c r="D61" s="85"/>
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="52">
-        <f>+'sirt-deformable-reg'!E63 - 'sirt-linear-deformable-reg'!E63</f>
-        <v>0</v>
-      </c>
+      <c r="D62" s="85"/>
     </row>
     <row r="63" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="52">
-        <f>+'sirt-deformable-reg'!E64 - 'sirt-linear-deformable-reg'!E64</f>
-        <v>0</v>
-      </c>
+      <c r="D63" s="85"/>
     </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="52">
-        <f>+'sirt-deformable-reg'!E65 - 'sirt-linear-deformable-reg'!E65</f>
-        <v>0</v>
-      </c>
+      <c r="D64" s="85"/>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="52">
-        <f>+'sirt-deformable-reg'!E66 - 'sirt-linear-deformable-reg'!E66</f>
-        <v>0</v>
-      </c>
+      <c r="D65" s="85"/>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" s="52">
-        <f>+'sirt-deformable-reg'!E67 - 'sirt-linear-deformable-reg'!E67</f>
-        <v>0</v>
-      </c>
+      <c r="D66" s="85"/>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" s="52">
-        <f>+'sirt-deformable-reg'!E68 - 'sirt-linear-deformable-reg'!E68</f>
-        <v>0</v>
-      </c>
+      <c r="D67" s="85"/>
     </row>
     <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68" s="52">
-        <f>+'sirt-deformable-reg'!E69 - 'sirt-linear-deformable-reg'!E69</f>
-        <v>0</v>
-      </c>
+      <c r="D68" s="85"/>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" s="52">
-        <f>+'sirt-deformable-reg'!E70 - 'sirt-linear-deformable-reg'!E70</f>
-        <v>0</v>
-      </c>
+      <c r="D69" s="85"/>
     </row>
     <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" s="52">
-        <f>+'sirt-deformable-reg'!E71 - 'sirt-linear-deformable-reg'!E71</f>
-        <v>0</v>
-      </c>
+      <c r="D70" s="85"/>
     </row>
     <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" s="52">
-        <f>+'sirt-deformable-reg'!E72 - 'sirt-linear-deformable-reg'!E72</f>
-        <v>0</v>
-      </c>
+      <c r="D71" s="85"/>
     </row>
     <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72" s="52">
-        <f>+'sirt-deformable-reg'!E73 - 'sirt-linear-deformable-reg'!E73</f>
-        <v>0</v>
-      </c>
+      <c r="D72" s="85"/>
     </row>
     <row r="73" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D73" s="52">
-        <f>+'sirt-deformable-reg'!E74 - 'sirt-linear-deformable-reg'!E74</f>
-        <v>0</v>
-      </c>
+      <c r="D73" s="85"/>
     </row>
     <row r="74" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D74" s="52">
-        <f>+'sirt-deformable-reg'!E75 - 'sirt-linear-deformable-reg'!E75</f>
-        <v>0</v>
-      </c>
+      <c r="D74" s="85"/>
     </row>
     <row r="75" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="52">
-        <f>+'sirt-deformable-reg'!E76 - 'sirt-linear-deformable-reg'!E76</f>
-        <v>0</v>
-      </c>
+      <c r="D75" s="85"/>
     </row>
     <row r="76" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D76" s="52">
-        <f>+'sirt-deformable-reg'!E77 - 'sirt-linear-deformable-reg'!E77</f>
-        <v>0</v>
-      </c>
+      <c r="D76" s="85"/>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D77" s="52">
-        <f>+'sirt-deformable-reg'!E78 - 'sirt-linear-deformable-reg'!E78</f>
-        <v>0</v>
-      </c>
+      <c r="D77" s="85"/>
     </row>
     <row r="78" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D78" s="52">
-        <f>+'sirt-deformable-reg'!E79 - 'sirt-linear-deformable-reg'!E79</f>
-        <v>0</v>
-      </c>
+      <c r="D78" s="85"/>
     </row>
     <row r="79" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D79" s="52">
-        <f>+'sirt-deformable-reg'!E80 - 'sirt-linear-deformable-reg'!E80</f>
-        <v>0</v>
-      </c>
+      <c r="D79" s="85"/>
     </row>
     <row r="80" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D80" s="52">
-        <f>+'sirt-deformable-reg'!E81 - 'sirt-linear-deformable-reg'!E81</f>
-        <v>0</v>
-      </c>
+      <c r="D80" s="85"/>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="52">
-        <f>+'sirt-deformable-reg'!E82 - 'sirt-linear-deformable-reg'!E82</f>
-        <v>0</v>
-      </c>
+      <c r="D81" s="85"/>
     </row>
     <row r="82" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D82" s="52">
-        <f>+'sirt-deformable-reg'!E83 - 'sirt-linear-deformable-reg'!E83</f>
-        <v>0</v>
-      </c>
+      <c r="D82" s="85"/>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="52">
-        <f>+'sirt-deformable-reg'!E84 - 'sirt-linear-deformable-reg'!E84</f>
-        <v>0</v>
-      </c>
+      <c r="D83" s="85"/>
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="52">
-        <f>+'sirt-deformable-reg'!E85 - 'sirt-linear-deformable-reg'!E85</f>
-        <v>0</v>
-      </c>
+      <c r="D84" s="85"/>
     </row>
     <row r="85" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="52">
-        <f>+'sirt-deformable-reg'!E86 - 'sirt-linear-deformable-reg'!E86</f>
-        <v>0</v>
-      </c>
+      <c r="D85" s="85"/>
     </row>
     <row r="86" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D86" s="52">
-        <f>+'sirt-deformable-reg'!E87 - 'sirt-linear-deformable-reg'!E87</f>
-        <v>0</v>
-      </c>
+      <c r="D86" s="85"/>
     </row>
     <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="52">
-        <f>+'sirt-deformable-reg'!E88 - 'sirt-linear-deformable-reg'!E88</f>
-        <v>0</v>
-      </c>
+      <c r="D87" s="85"/>
     </row>
     <row r="88" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="52">
-        <f>+'sirt-deformable-reg'!E89 - 'sirt-linear-deformable-reg'!E89</f>
-        <v>0</v>
-      </c>
+      <c r="D88" s="85"/>
     </row>
     <row r="89" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="52">
-        <f>+'sirt-deformable-reg'!E90 - 'sirt-linear-deformable-reg'!E90</f>
-        <v>0</v>
-      </c>
+      <c r="D89" s="85"/>
     </row>
     <row r="90" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="52">
-        <f>+'sirt-deformable-reg'!E91 - 'sirt-linear-deformable-reg'!E91</f>
-        <v>0</v>
-      </c>
+      <c r="D90" s="85"/>
     </row>
     <row r="91" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="52">
-        <f>+'sirt-deformable-reg'!E92 - 'sirt-linear-deformable-reg'!E92</f>
-        <v>0</v>
-      </c>
+      <c r="D91" s="85"/>
     </row>
     <row r="92" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="52">
-        <f>+'sirt-deformable-reg'!E93 - 'sirt-linear-deformable-reg'!E93</f>
-        <v>0</v>
-      </c>
+      <c r="D92" s="85"/>
     </row>
     <row r="93" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D93" s="52">
-        <f>+'sirt-deformable-reg'!E94 - 'sirt-linear-deformable-reg'!E94</f>
-        <v>0</v>
-      </c>
+      <c r="D93" s="85"/>
     </row>
     <row r="94" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="52">
-        <f>+'sirt-deformable-reg'!E95 - 'sirt-linear-deformable-reg'!E95</f>
-        <v>0</v>
-      </c>
+      <c r="D94" s="85"/>
     </row>
     <row r="95" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="52">
-        <f>+'sirt-deformable-reg'!E96 - 'sirt-linear-deformable-reg'!E96</f>
-        <v>0</v>
-      </c>
+      <c r="D95" s="85"/>
     </row>
     <row r="96" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="52">
-        <f>+'sirt-deformable-reg'!E97 - 'sirt-linear-deformable-reg'!E97</f>
-        <v>0</v>
-      </c>
+      <c r="D96" s="85"/>
     </row>
     <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="52">
-        <f>+'sirt-deformable-reg'!E98 - 'sirt-linear-deformable-reg'!E98</f>
-        <v>0</v>
-      </c>
+      <c r="D97" s="85"/>
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D98" s="52">
-        <f>+'sirt-deformable-reg'!E99 - 'sirt-linear-deformable-reg'!E99</f>
-        <v>0</v>
-      </c>
+      <c r="D98" s="85"/>
     </row>
     <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="52">
-        <f>+'sirt-deformable-reg'!E100 - 'sirt-linear-deformable-reg'!E100</f>
-        <v>0</v>
-      </c>
+      <c r="D99" s="85"/>
     </row>
     <row r="100" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D100" s="52">
-        <f>+'sirt-deformable-reg'!E101 - 'sirt-linear-deformable-reg'!E101</f>
-        <v>0</v>
-      </c>
+      <c r="D100" s="85"/>
     </row>
     <row r="101" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D101" s="52">
-        <f>+'sirt-deformable-reg'!E102 - 'sirt-linear-deformable-reg'!E102</f>
-        <v>0</v>
-      </c>
+      <c r="D101" s="85"/>
     </row>
     <row r="102" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="52">
-        <f>+'sirt-deformable-reg'!E103 - 'sirt-linear-deformable-reg'!E103</f>
-        <v>0</v>
-      </c>
+      <c r="D102" s="85"/>
     </row>
     <row r="103" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D103" s="52">
-        <f>+'sirt-deformable-reg'!E104 - 'sirt-linear-deformable-reg'!E104</f>
-        <v>0</v>
-      </c>
+      <c r="D103" s="85"/>
     </row>
     <row r="104" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D104" s="52">
-        <f>+'sirt-deformable-reg'!E105 - 'sirt-linear-deformable-reg'!E105</f>
-        <v>0</v>
-      </c>
+      <c r="D104" s="85"/>
     </row>
     <row r="105" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D105" s="52">
-        <f>+'sirt-deformable-reg'!E106 - 'sirt-linear-deformable-reg'!E106</f>
-        <v>0</v>
-      </c>
+      <c r="D105" s="85"/>
     </row>
     <row r="106" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D106" s="52">
-        <f>+'sirt-deformable-reg'!E107 - 'sirt-linear-deformable-reg'!E107</f>
-        <v>0</v>
-      </c>
+      <c r="D106" s="85"/>
     </row>
     <row r="107" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D107" s="52">
-        <f>+'sirt-deformable-reg'!E108 - 'sirt-linear-deformable-reg'!E108</f>
-        <v>0</v>
-      </c>
+      <c r="D107" s="85"/>
     </row>
     <row r="108" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D108" s="52">
-        <f>+'sirt-deformable-reg'!E109 - 'sirt-linear-deformable-reg'!E109</f>
-        <v>0</v>
-      </c>
+      <c r="D108" s="85"/>
     </row>
     <row r="109" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D109" s="52">
-        <f>+'sirt-deformable-reg'!E110 - 'sirt-linear-deformable-reg'!E110</f>
-        <v>0</v>
-      </c>
+      <c r="D109" s="85"/>
     </row>
     <row r="110" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D110" s="52">
-        <f>+'sirt-deformable-reg'!E111 - 'sirt-linear-deformable-reg'!E111</f>
-        <v>0</v>
-      </c>
+      <c r="D110" s="85"/>
     </row>
     <row r="111" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D111" s="52">
-        <f>+'sirt-deformable-reg'!E112 - 'sirt-linear-deformable-reg'!E112</f>
-        <v>0</v>
-      </c>
+      <c r="D111" s="85"/>
     </row>
     <row r="112" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D112" s="52">
-        <f>+'sirt-deformable-reg'!E113 - 'sirt-linear-deformable-reg'!E113</f>
-        <v>0</v>
-      </c>
+      <c r="D112" s="85"/>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D113" s="52">
-        <f>+'sirt-deformable-reg'!E114 - 'sirt-linear-deformable-reg'!E114</f>
-        <v>0</v>
-      </c>
+      <c r="D113" s="85"/>
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D114" s="52">
-        <f>+'sirt-deformable-reg'!E115 - 'sirt-linear-deformable-reg'!E115</f>
-        <v>0</v>
-      </c>
+      <c r="D114" s="85"/>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D115" s="52">
-        <f>+'sirt-deformable-reg'!E116 - 'sirt-linear-deformable-reg'!E116</f>
-        <v>0</v>
-      </c>
+      <c r="D115" s="85"/>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D116" s="52">
-        <f>+'sirt-deformable-reg'!E117 - 'sirt-linear-deformable-reg'!E117</f>
-        <v>0</v>
-      </c>
+      <c r="D116" s="85"/>
     </row>
     <row r="117" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D117" s="52">
-        <f>+'sirt-deformable-reg'!E118 - 'sirt-linear-deformable-reg'!E118</f>
-        <v>0</v>
-      </c>
+      <c r="D117" s="85"/>
     </row>
     <row r="118" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D118" s="52">
-        <f>+'sirt-deformable-reg'!E119 - 'sirt-linear-deformable-reg'!E119</f>
-        <v>0</v>
-      </c>
+      <c r="D118" s="85"/>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D119" s="52">
-        <f>+'sirt-deformable-reg'!E120 - 'sirt-linear-deformable-reg'!E120</f>
-        <v>0</v>
-      </c>
+      <c r="D119" s="85"/>
     </row>
     <row r="120" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D120" s="52">
-        <f>+'sirt-deformable-reg'!E121 - 'sirt-linear-deformable-reg'!E121</f>
-        <v>0</v>
-      </c>
+      <c r="D120" s="85"/>
     </row>
     <row r="121" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D121" s="52">
-        <f>+'sirt-deformable-reg'!E122 - 'sirt-linear-deformable-reg'!E122</f>
-        <v>0</v>
-      </c>
+      <c r="D121" s="85"/>
     </row>
     <row r="122" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D122" s="52">
-        <f>+'sirt-deformable-reg'!E123 - 'sirt-linear-deformable-reg'!E123</f>
-        <v>0</v>
-      </c>
+      <c r="D122" s="85"/>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D123" s="52">
-        <f>+'sirt-deformable-reg'!E124 - 'sirt-linear-deformable-reg'!E124</f>
-        <v>0</v>
-      </c>
+      <c r="D123" s="85"/>
     </row>
     <row r="124" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D124" s="52">
-        <f>+'sirt-deformable-reg'!E125 - 'sirt-linear-deformable-reg'!E125</f>
-        <v>0</v>
-      </c>
+      <c r="D124" s="85"/>
     </row>
     <row r="125" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D125" s="52">
-        <f>+'sirt-deformable-reg'!E126 - 'sirt-linear-deformable-reg'!E126</f>
-        <v>0</v>
-      </c>
+      <c r="D125" s="85"/>
     </row>
     <row r="126" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D126" s="52">
-        <f>+'sirt-deformable-reg'!E127 - 'sirt-linear-deformable-reg'!E127</f>
-        <v>0</v>
-      </c>
+      <c r="D126" s="85"/>
     </row>
     <row r="127" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D127" s="52">
-        <f>+'sirt-deformable-reg'!E128 - 'sirt-linear-deformable-reg'!E128</f>
-        <v>0</v>
-      </c>
+      <c r="D127" s="85"/>
     </row>
     <row r="128" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D128" s="52">
-        <f>+'sirt-deformable-reg'!E129 - 'sirt-linear-deformable-reg'!E129</f>
-        <v>0</v>
-      </c>
+      <c r="D128" s="85"/>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D129" s="52">
-        <f>+'sirt-deformable-reg'!E130 - 'sirt-linear-deformable-reg'!E130</f>
-        <v>0</v>
-      </c>
+      <c r="D129" s="85"/>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D130" s="52">
-        <f>+'sirt-deformable-reg'!E131 - 'sirt-linear-deformable-reg'!E131</f>
-        <v>0</v>
-      </c>
+      <c r="D130" s="85"/>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D131" s="52">
-        <f>+'sirt-deformable-reg'!E132 - 'sirt-linear-deformable-reg'!E132</f>
-        <v>0</v>
-      </c>
+      <c r="D131" s="85"/>
     </row>
     <row r="132" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D132" s="52">
-        <f>+'sirt-deformable-reg'!E133 - 'sirt-linear-deformable-reg'!E133</f>
-        <v>0</v>
-      </c>
+      <c r="D132" s="85"/>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D133" s="52">
-        <f>+'sirt-deformable-reg'!E134 - 'sirt-linear-deformable-reg'!E134</f>
-        <v>0</v>
-      </c>
+      <c r="D133" s="85"/>
     </row>
     <row r="134" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D134" s="52">
-        <f>+'sirt-deformable-reg'!E135 - 'sirt-linear-deformable-reg'!E135</f>
-        <v>0</v>
-      </c>
+      <c r="D134" s="85"/>
     </row>
     <row r="135" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D135" s="52">
-        <f>+'sirt-deformable-reg'!E136 - 'sirt-linear-deformable-reg'!E136</f>
-        <v>0</v>
-      </c>
+      <c r="D135" s="85"/>
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D136" s="52">
-        <f>+'sirt-deformable-reg'!E137 - 'sirt-linear-deformable-reg'!E137</f>
-        <v>0</v>
-      </c>
+      <c r="D136" s="85"/>
     </row>
     <row r="137" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D137" s="52">
-        <f>+'sirt-deformable-reg'!E138 - 'sirt-linear-deformable-reg'!E138</f>
-        <v>0</v>
-      </c>
+      <c r="D137" s="85"/>
     </row>
     <row r="138" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D138" s="52">
-        <f>+'sirt-deformable-reg'!E139 - 'sirt-linear-deformable-reg'!E139</f>
-        <v>0</v>
-      </c>
+      <c r="D138" s="85"/>
     </row>
     <row r="139" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D139" s="52">
-        <f>+'sirt-deformable-reg'!E140 - 'sirt-linear-deformable-reg'!E140</f>
-        <v>0</v>
-      </c>
+      <c r="D139" s="85"/>
     </row>
     <row r="140" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D140" s="52">
-        <f>+'sirt-deformable-reg'!E141 - 'sirt-linear-deformable-reg'!E141</f>
-        <v>0</v>
-      </c>
+      <c r="D140" s="85"/>
     </row>
     <row r="141" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D141" s="52">
-        <f>+'sirt-deformable-reg'!E142 - 'sirt-linear-deformable-reg'!E142</f>
-        <v>0</v>
-      </c>
+      <c r="D141" s="85"/>
     </row>
     <row r="142" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D142" s="52">
-        <f>+'sirt-deformable-reg'!E143 - 'sirt-linear-deformable-reg'!E143</f>
-        <v>0</v>
-      </c>
+      <c r="D142" s="85"/>
     </row>
     <row r="143" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D143" s="52">
-        <f>+'sirt-deformable-reg'!E144 - 'sirt-linear-deformable-reg'!E144</f>
-        <v>0</v>
-      </c>
+      <c r="D143" s="85"/>
     </row>
     <row r="144" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D144" s="52">
-        <f>+'sirt-deformable-reg'!E145 - 'sirt-linear-deformable-reg'!E145</f>
-        <v>0</v>
-      </c>
+      <c r="D144" s="85"/>
     </row>
     <row r="145" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D145" s="52">
-        <f>+'sirt-deformable-reg'!E146 - 'sirt-linear-deformable-reg'!E146</f>
-        <v>0</v>
-      </c>
+      <c r="D145" s="85"/>
     </row>
     <row r="146" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D146" s="52">
-        <f>+'sirt-deformable-reg'!E147 - 'sirt-linear-deformable-reg'!E147</f>
-        <v>0</v>
-      </c>
+      <c r="D146" s="85"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147" s="85"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:I4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>